<commit_message>
Code outputs single gene deletion table. Switched to E coli model
</commit_message>
<xml_diff>
--- a/toy_data_output.xlsx
+++ b/toy_data_output.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\pythonScripts\Mtb_inhibition\Mtb_inhibition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A01862-78D7-462C-BC7B-33908696AF9F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F88A6CE-E3CE-470E-9EC9-9B7C31EC4B1A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" xr2:uid="{D0B9BDEA-F22B-4D75-9D82-650F222F8BFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -6903,8 +6904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{410BC57F-53AD-4BF7-86BF-8529DBC463AB}">
   <dimension ref="A1:G1486"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -47046,7 +47047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53865A3-CF5E-48F5-B3A8-CC6C4B7037AE}">
   <dimension ref="B1:D824"/>
   <sheetViews>
-    <sheetView topLeftCell="A798" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D660" sqref="D660"/>
     </sheetView>
   </sheetViews>
@@ -55508,4 +55509,16 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF92BBB8-F5E5-45DA-9B8F-80F02E0AF51E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>